<commit_message>
Änderung Histogramm statt Scatter
</commit_message>
<xml_diff>
--- a/assets/Zufriedenheit-cleaned.xlsx
+++ b/assets/Zufriedenheit-cleaned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhgraubuenden-my.sharepoint.com/personal/nyffeltamara_fhgr_ch/Documents/PY-Skriptesammlung/FHGR_Data_Visualization/02_DaDe_Zufriedenheits_Dashboard/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55d6cdc912bf3ef8/Dokumente/GitHub/Dashboard_Design/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="8_{EABC2878-4134-421C-8096-C3030AEA7CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EADA036-C094-4BF6-BCEE-68F7B396EAD0}"/>
+  <xr:revisionPtr revIDLastSave="353" documentId="8_{EABC2878-4134-421C-8096-C3030AEA7CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA167090-D7D5-4407-9296-83086506F7FA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{807A4729-B974-43DF-9F85-699DD16C51D8}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="24">
   <si>
     <t>Jahr</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>65 Jahre +</t>
+  </si>
+  <si>
+    <t>Zusammenleben</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -259,10 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3172,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5028D925-7BF8-434F-99D4-BBA3B585A086}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E113" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3202,7 +3204,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -11161,7 +11163,7 @@
       <c r="A3" s="16">
         <v>2007</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -11200,7 +11202,7 @@
       <c r="A4" s="16">
         <v>2007</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -11241,7 +11243,7 @@
       <c r="A5" s="16">
         <v>2007</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="16" t="s">

</xml_diff>